<commit_message>
CREATE NOTES on THEORY OF THE LEARNABLE
</commit_message>
<xml_diff>
--- a/a_super_harsh_guide_to_machine_learning.xlsx
+++ b/a_super_harsh_guide_to_machine_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17328\Desktop\A-Super-Harsh-Guide-to-Machine-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792A7321-324E-4ACB-951E-8D88BDF5C5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED9790F-1E45-4431-975C-62E927EC5080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC5C0398-6584-4145-8E96-7FDAF871F3BD}"/>
   </bookViews>
@@ -466,7 +466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +487,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -528,6 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -846,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C675B78-0CCB-4951-82FE-89881C2CD1F9}">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +942,7 @@
       <c r="H4" s="1">
         <v>44884</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
@@ -959,7 +966,7 @@
       <c r="L6" s="1">
         <v>44884</v>
       </c>
-      <c r="M6" s="2"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
@@ -971,7 +978,7 @@
       <c r="L7" s="1">
         <v>44885</v>
       </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J8" t="s">

</xml_diff>